<commit_message>
All contact Persons details added
</commit_message>
<xml_diff>
--- a/Email-Automation-Bot/Project_Data.xlsx
+++ b/Email-Automation-Bot/Project_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5469e9f4aa070a41/Documents/UiPath/ReadExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leorw\University\IF300\SE762-IS300-Project\Email-Automation-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D70D1221-3408-4F3B-8BE8-F234245FF6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A816ADB8-2B3E-4C78-974C-3C2853C0333E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71374CC-BEE5-492D-8594-0E3B222F1355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3825" yWindow="3660" windowWidth="33675" windowHeight="16770" xr2:uid="{35F2FEA0-FCB0-43AF-A617-1082C65B0A32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{35F2FEA0-FCB0-43AF-A617-1082C65B0A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="84">
   <si>
     <t>Project Category</t>
   </si>
@@ -238,6 +238,54 @@
   </si>
   <si>
     <t>AlsetTest</t>
+  </si>
+  <si>
+    <t>Parrot email</t>
+  </si>
+  <si>
+    <t>Alstef email</t>
+  </si>
+  <si>
+    <t>Vista email</t>
+  </si>
+  <si>
+    <t>4 email</t>
+  </si>
+  <si>
+    <t>Parrot Name 2</t>
+  </si>
+  <si>
+    <t>Parrot Name 3</t>
+  </si>
+  <si>
+    <t>Parrot Email 2</t>
+  </si>
+  <si>
+    <t>Parrot Email 3</t>
+  </si>
+  <si>
+    <t>Alstef Email 2</t>
+  </si>
+  <si>
+    <t>Alstef 3</t>
+  </si>
+  <si>
+    <t>Lancom email 1</t>
+  </si>
+  <si>
+    <t>Lancom name 3</t>
+  </si>
+  <si>
+    <t>Beckhoff email 1</t>
+  </si>
+  <si>
+    <t>Beckoff person 1</t>
+  </si>
+  <si>
+    <t>Air nz Name 2</t>
+  </si>
+  <si>
+    <t>Crown email 3</t>
   </si>
 </sst>
 </file>
@@ -781,7 +829,7 @@
   <dimension ref="A1:AB996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,27 +969,27 @@
         <v>66</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>62</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="10" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>62</v>
@@ -973,7 +1021,7 @@
         <v>67</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>62</v>
@@ -983,17 +1031,17 @@
         <v>60</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>62</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>62</v>
@@ -1025,7 +1073,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>62</v>
@@ -1077,7 +1125,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>62</v>
@@ -1285,7 +1333,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>62</v>
@@ -1302,7 +1350,7 @@
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="M10" s="10" t="s">
         <v>61</v>
@@ -1409,7 +1457,7 @@
         <v>60</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>62</v>
@@ -1604,7 +1652,7 @@
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>61</v>
@@ -1854,10 +1902,10 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Rewrote entire reading of excel data logic to make it work with sanitised data so that the headers of the source sheet don't make it difficult to manipulate the data.
</commit_message>
<xml_diff>
--- a/Email-Automation-Bot/Project_Data.xlsx
+++ b/Email-Automation-Bot/Project_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leorw\University\IF300\SE762-IS300-Project\Email-Automation-Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Softeng762\Email-Automation-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71374CC-BEE5-492D-8594-0E3B222F1355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3381778C-5FE8-41F2-8C72-03CCB806F407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{35F2FEA0-FCB0-43AF-A617-1082C65B0A32}"/>
+    <workbookView xWindow="-28920" yWindow="2595" windowWidth="29040" windowHeight="15840" xr2:uid="{35F2FEA0-FCB0-43AF-A617-1082C65B0A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -829,7 +829,7 @@
   <dimension ref="A1:AB996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,9 @@
       <c r="B3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" s="10" t="s">
         <v>66</v>
       </c>
@@ -1016,7 +1018,9 @@
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
       <c r="D4" s="10" t="s">
         <v>67</v>
       </c>
@@ -1068,7 +1072,9 @@
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
       <c r="D5" s="10" t="s">
         <v>60</v>
       </c>
@@ -1120,7 +1126,9 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
       <c r="D6" s="10" t="s">
         <v>60</v>
       </c>
@@ -1172,7 +1180,9 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
       <c r="D7" s="10" t="s">
         <v>60</v>
       </c>
@@ -1224,7 +1234,9 @@
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
       <c r="D8" s="10" t="s">
         <v>60</v>
       </c>

</xml_diff>